<commit_message>
update docs and add more
</commit_message>
<xml_diff>
--- a/Kube cluster on R710.xlsx
+++ b/Kube cluster on R710.xlsx
@@ -113,9 +113,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>ks1</t>
   </si>
   <si>
@@ -249,6 +246,9 @@
   </si>
   <si>
     <t xml:space="preserve"> (from google search: terraform on premise kubernetes )</t>
+  </si>
+  <si>
+    <t>dev1</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -324,6 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -651,7 +652,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,7 +666,7 @@
         <v>2</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
@@ -678,7 +679,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -694,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -708,7 +709,7 @@
     <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="P4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -724,7 +725,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -738,7 +739,7 @@
     <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="P6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -754,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -805,10 +806,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -830,18 +831,18 @@
         <v>22</v>
       </c>
       <c r="O11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -855,19 +856,19 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
       </c>
       <c r="L13">
         <v>176</v>
       </c>
       <c r="N13">
-        <v>1000</v>
+        <v>930</v>
       </c>
       <c r="P13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -875,21 +876,21 @@
         <v>25</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14">
         <f>F11-E14</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2</v>
       </c>
       <c r="I14">
         <f>I11-H14</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14">
         <v>20</v>
@@ -900,22 +901,22 @@
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N23" si="1">N13-M14</f>
-        <v>1000</v>
+        <v>930</v>
       </c>
       <c r="P14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S14" t="s">
+        <v>38</v>
+      </c>
+      <c r="T14" t="s">
         <v>39</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>40</v>
       </c>
-      <c r="U14" t="s">
-        <v>41</v>
-      </c>
       <c r="V14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -923,21 +924,21 @@
         <v>26</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <f t="shared" ref="F15:F17" si="2">F14-E15</f>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="H15" s="6">
+        <v>2</v>
       </c>
       <c r="I15">
         <f t="shared" ref="I15:I23" si="3">I14-H15</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K15">
         <v>20</v>
@@ -948,7 +949,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>930</v>
       </c>
       <c r="P15">
         <v>203</v>
@@ -959,21 +960,21 @@
         <v>27</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="H16" s="6">
+        <v>2</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K16">
         <v>20</v>
@@ -984,7 +985,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>930</v>
       </c>
       <c r="P16">
         <v>204</v>
@@ -998,31 +999,31 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M17">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N17">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>630</v>
       </c>
       <c r="P17">
         <v>205</v>
@@ -1033,31 +1034,31 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H18">
         <v>4</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M18">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N18">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>330</v>
       </c>
       <c r="P18">
         <v>206</v>
@@ -1068,28 +1069,28 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19">
         <v>4</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M19">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="P19">
         <v>207</v>
@@ -1104,21 +1105,21 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -1131,21 +1132,21 @@
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="P21" s="3"/>
     </row>
@@ -1158,27 +1159,27 @@
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -1188,24 +1189,31 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="H23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="K23">
+        <v>80</v>
+      </c>
+      <c r="L23">
+        <f>L16-K23</f>
+        <v>36</v>
+      </c>
       <c r="N23">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="P23">
         <v>208</v>
       </c>
       <c r="R23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -1253,65 +1261,65 @@
       </c>
       <c r="H32" s="3"/>
       <c r="T32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U52" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ubuntu workstation setup
plus rename files so they show in order
</commit_message>
<xml_diff>
--- a/Kube cluster on R710.xlsx
+++ b/Kube cluster on R710.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>GB</t>
   </si>
@@ -249,13 +249,16 @@
   </si>
   <si>
     <t>dev1</t>
+  </si>
+  <si>
+    <t>Proxmox uses 8GB for swap !!! + OS ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +286,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -315,7 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -325,6 +336,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -652,7 +664,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,6 +782,11 @@
       <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
       <c r="F9" t="s">
         <v>6</v>
       </c>
@@ -816,12 +833,12 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="E11">
-        <v>4</v>
+      <c r="E11" s="7">
+        <v>10</v>
       </c>
       <c r="F11">
         <f t="shared" ref="F11:F23" si="0">F10-E11</f>
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -880,7 +897,7 @@
       </c>
       <c r="F14">
         <f>F11-E14</f>
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
         <v>29</v>
@@ -893,11 +910,11 @@
         <v>20</v>
       </c>
       <c r="K14">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L14">
         <f>L13-K14</f>
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N23" si="1">N13-M14</f>
@@ -928,7 +945,7 @@
       </c>
       <c r="F15">
         <f t="shared" ref="F15:F17" si="2">F14-E15</f>
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>30</v>
@@ -941,11 +958,11 @@
         <v>18</v>
       </c>
       <c r="K15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L15">
         <f>L14-K15</f>
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
@@ -964,7 +981,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>31</v>
@@ -977,11 +994,11 @@
         <v>16</v>
       </c>
       <c r="K16">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L16">
         <f>L15-K16</f>
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
@@ -999,11 +1016,11 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
         <v>32</v>
@@ -1034,11 +1051,11 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
@@ -1069,7 +1086,7 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1203,7 +1220,7 @@
       </c>
       <c r="L23">
         <f>L16-K23</f>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="N23">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update, add more info
</commit_message>
<xml_diff>
--- a/Kube cluster on R710.xlsx
+++ b/Kube cluster on R710.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>GB</t>
   </si>
@@ -155,9 +155,6 @@
     <t>fix at 192.168.124.202</t>
   </si>
   <si>
-    <t>Dev Main + Database + docker containers + S3</t>
-  </si>
-  <si>
     <t>rest for OS images +</t>
   </si>
   <si>
@@ -252,6 +249,18 @@
   </si>
   <si>
     <t>Proxmox uses 8GB for swap !!! + OS ?</t>
+  </si>
+  <si>
+    <t>Dev Main + Database + docker containers</t>
+  </si>
+  <si>
+    <t>load1</t>
+  </si>
+  <si>
+    <t>NGINX load balancer for k3s servers</t>
+  </si>
+  <si>
+    <t>Don’t use this worker:</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +318,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -337,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,7 +680,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
@@ -691,7 +707,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -707,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
@@ -721,7 +737,7 @@
     <row r="4" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="P4" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -737,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
@@ -751,7 +767,7 @@
     <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="P6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
@@ -767,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -783,7 +799,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -823,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -848,18 +864,18 @@
         <v>22</v>
       </c>
       <c r="O11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
         <v>28</v>
@@ -873,10 +889,10 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
       </c>
       <c r="L13">
         <v>176</v>
@@ -1015,25 +1031,25 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
-        <v>6</v>
+      <c r="E17" s="8">
+        <v>7</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
         <v>32</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M17">
         <v>300</v>
@@ -1050,25 +1066,25 @@
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>6</v>
+      <c r="E18" s="8">
+        <v>7</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
         <v>33</v>
       </c>
       <c r="H18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M18">
         <v>300</v>
@@ -1082,32 +1098,33 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
       <c r="D19">
         <v>3</v>
       </c>
-      <c r="E19">
-        <v>6</v>
-      </c>
+      <c r="E19" s="8"/>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
         <v>34</v>
       </c>
-      <c r="H19">
-        <v>4</v>
+      <c r="H19" s="8">
+        <v>0</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="M19">
-        <v>300</v>
+        <v>6</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0</v>
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="P19">
         <v>207</v>
@@ -1119,7 +1136,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
         <v>35</v>
@@ -1129,14 +1146,14 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="P20" s="3"/>
     </row>
@@ -1146,7 +1163,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>36</v>
@@ -1156,14 +1173,14 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="P21" s="3"/>
     </row>
@@ -1173,7 +1190,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
         <v>37</v>
@@ -1183,54 +1200,89 @@
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>330</v>
       </c>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23">
+        <v>75</v>
+      </c>
+      <c r="E23" s="8">
         <v>8</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23">
+        <v>73</v>
+      </c>
+      <c r="H23" s="8">
         <v>4</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>80</v>
+        <v>2</v>
+      </c>
+      <c r="K23" s="8">
+        <v>0</v>
       </c>
       <c r="L23">
         <f>L16-K23</f>
-        <v>21</v>
+        <v>101</v>
+      </c>
+      <c r="M23" s="8">
+        <v>200</v>
       </c>
       <c r="N23">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="P23">
         <v>208</v>
       </c>
       <c r="R23" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="8">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24" si="4">F23-E24</f>
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" ref="I24" si="5">I23-H24</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="8">
+        <v>25</v>
+      </c>
+      <c r="L24">
+        <f>L23-K24</f>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
@@ -1278,65 +1330,65 @@
       </c>
       <c r="H32" s="3"/>
       <c r="T32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="20:21" x14ac:dyDescent="0.3">
       <c r="T37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="20:21" x14ac:dyDescent="0.3">
       <c r="U48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="21:21" x14ac:dyDescent="0.3">
       <c r="U52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>